<commit_message>
update round 2 move list to account for movement
</commit_message>
<xml_diff>
--- a/assets/Dungeon Move List.xlsx
+++ b/assets/Dungeon Move List.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\GitHub\raidnight\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Template" sheetId="1" r:id="rId3"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="9">
   <si>
     <t>TailSwipe</t>
   </si>
@@ -33,25 +41,34 @@
   <si>
     <t>SpikeTrap</t>
   </si>
+  <si>
+    <t>Move:down</t>
+  </si>
+  <si>
+    <t>Move:up</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -79,53 +96,314 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D300"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -136,7 +414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -147,7 +425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -158,18 +436,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -180,7 +458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -191,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -202,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -213,7 +491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -221,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -235,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -246,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -257,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -268,18 +546,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -290,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -301,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -312,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -323,7 +601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -331,10 +609,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -345,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -356,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
@@ -367,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -378,18 +656,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -480,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,18 +769,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,10 +832,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>3</v>
       </c>
@@ -590,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,18 +879,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,10 +942,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
@@ -703,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,18 +992,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,7 +1014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +1069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>3</v>
       </c>
@@ -813,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,18 +1102,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +1124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +1135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +1146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +1157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,7 +1190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -923,7 +1201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,18 +1212,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -1000,10 +1278,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,18 +1325,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,10 +1388,10 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,18 +1435,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,7 +1490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,10 +1498,10 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,18 +1548,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -1333,10 +1611,10 @@
         <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>3</v>
       </c>
@@ -1369,7 +1647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,18 +1658,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -1413,7 +1691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -1443,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -1457,7 +1735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>3</v>
       </c>
@@ -1479,7 +1757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,18 +1768,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -1556,10 +1834,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>0</v>
       </c>
@@ -1581,7 +1859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>3</v>
       </c>
@@ -1592,7 +1870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,18 +1881,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,10 +1944,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -1691,7 +1969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>0</v>
       </c>
@@ -1713,18 +1991,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +2013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +2024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +2035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +2046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>0</v>
       </c>
@@ -1776,10 +2054,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +2071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>0</v>
       </c>
@@ -1804,7 +2082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>3</v>
       </c>
@@ -1815,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,18 +2104,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +2137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>0</v>
       </c>
@@ -1870,7 +2148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +2159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>0</v>
       </c>
@@ -1889,10 +2167,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="160">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
@@ -1903,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +2192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>3</v>
       </c>
@@ -1925,7 +2203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -1936,18 +2214,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -1958,7 +2236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +2258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>0</v>
       </c>
@@ -1991,7 +2269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>0</v>
       </c>
@@ -1999,10 +2277,10 @@
         <v>1</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="170">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>3</v>
       </c>
@@ -2035,7 +2313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>0</v>
       </c>
@@ -2046,18 +2324,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>0</v>
       </c>
@@ -2082,7 +2360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>0</v>
       </c>
@@ -2112,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="180">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +2404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>0</v>
       </c>
@@ -2137,7 +2415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>3</v>
       </c>
@@ -2148,7 +2426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,18 +2437,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>0</v>
       </c>
@@ -2181,7 +2459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>0</v>
       </c>
@@ -2192,7 +2470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>0</v>
       </c>
@@ -2203,7 +2481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>0</v>
       </c>
@@ -2214,7 +2492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>0</v>
       </c>
@@ -2222,10 +2500,10 @@
         <v>1</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="190">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +2525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>3</v>
       </c>
@@ -2258,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>0</v>
       </c>
@@ -2269,18 +2547,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +2569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>0</v>
       </c>
@@ -2332,10 +2610,10 @@
         <v>1</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>0</v>
       </c>
@@ -2349,7 +2627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>3</v>
       </c>
@@ -2371,7 +2649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>0</v>
       </c>
@@ -2382,18 +2660,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>0</v>
       </c>
@@ -2415,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>0</v>
       </c>
@@ -2445,10 +2723,10 @@
         <v>1</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="210">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>0</v>
       </c>
@@ -2459,7 +2737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>3</v>
       </c>
@@ -2481,7 +2759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>0</v>
       </c>
@@ -2492,18 +2770,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>0</v>
       </c>
@@ -2514,7 +2792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>0</v>
       </c>
@@ -2536,7 +2814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>0</v>
       </c>
@@ -2547,7 +2825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>0</v>
       </c>
@@ -2555,10 +2833,10 @@
         <v>1</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>0</v>
       </c>
@@ -2580,7 +2858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>3</v>
       </c>
@@ -2591,7 +2869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>0</v>
       </c>
@@ -2602,18 +2880,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>0</v>
       </c>
@@ -2627,7 +2905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>0</v>
       </c>
@@ -2660,7 +2938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>0</v>
       </c>
@@ -2668,10 +2946,10 @@
         <v>1</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="230">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>0</v>
       </c>
@@ -2693,7 +2971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>3</v>
       </c>
@@ -2704,7 +2982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>0</v>
       </c>
@@ -2715,18 +2993,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +3015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +3026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +3037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +3048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>0</v>
       </c>
@@ -2778,10 +3056,10 @@
         <v>1</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="240">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +3070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +3081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>3</v>
       </c>
@@ -2814,7 +3092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>0</v>
       </c>
@@ -2825,18 +3103,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +3125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +3136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +3147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +3158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>0</v>
       </c>
@@ -2888,10 +3166,10 @@
         <v>1</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="250">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>0</v>
       </c>
@@ -2905,7 +3183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>0</v>
       </c>
@@ -2916,7 +3194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>3</v>
       </c>
@@ -2927,7 +3205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>0</v>
       </c>
@@ -2938,18 +3216,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>0</v>
       </c>
@@ -2960,7 +3238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>0</v>
       </c>
@@ -2971,7 +3249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>0</v>
       </c>
@@ -2982,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>0</v>
       </c>
@@ -2993,7 +3271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>0</v>
       </c>
@@ -3001,10 +3279,10 @@
         <v>1</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="260">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>0</v>
       </c>
@@ -3015,7 +3293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>0</v>
       </c>
@@ -3026,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>3</v>
       </c>
@@ -3037,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>0</v>
       </c>
@@ -3048,18 +3326,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>0</v>
       </c>
@@ -3070,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>0</v>
       </c>
@@ -3092,7 +3370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>0</v>
       </c>
@@ -3103,7 +3381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>0</v>
       </c>
@@ -3111,10 +3389,10 @@
         <v>1</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="270">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>0</v>
       </c>
@@ -3125,7 +3403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>0</v>
       </c>
@@ -3136,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>3</v>
       </c>
@@ -3147,7 +3425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>0</v>
       </c>
@@ -3158,18 +3436,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +3461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>0</v>
       </c>
@@ -3194,7 +3472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>0</v>
       </c>
@@ -3205,7 +3483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>0</v>
       </c>
@@ -3216,7 +3494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>0</v>
       </c>
@@ -3224,10 +3502,10 @@
         <v>1</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>0</v>
       </c>
@@ -3238,7 +3516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>0</v>
       </c>
@@ -3249,7 +3527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>3</v>
       </c>
@@ -3260,7 +3538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>0</v>
       </c>
@@ -3271,18 +3549,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>0</v>
       </c>
@@ -3293,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>0</v>
       </c>
@@ -3304,7 +3582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>0</v>
       </c>
@@ -3315,7 +3593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>0</v>
       </c>
@@ -3334,10 +3612,10 @@
         <v>1</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="290">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>0</v>
       </c>
@@ -3348,7 +3626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>0</v>
       </c>
@@ -3359,7 +3637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>3</v>
       </c>
@@ -3370,7 +3648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>0</v>
       </c>
@@ -3381,18 +3659,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>0</v>
       </c>
@@ -3403,7 +3681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>0</v>
       </c>
@@ -3414,7 +3692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
         <v>0</v>
       </c>
@@ -3425,7 +3703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>0</v>
       </c>
@@ -3436,7 +3714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>0</v>
       </c>
@@ -3444,10 +3722,10 @@
         <v>1</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="300">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>0</v>
       </c>
@@ -3462,6 +3740,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>